<commit_message>
refatoração - cálculos de apoio médio
</commit_message>
<xml_diff>
--- a/analises/2023/analise_descritiva/dados/aon-genero.xlsx
+++ b/analises/2023/analise_descritiva/dados/aon-genero.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>modalidade</t>
   </si>
@@ -37,25 +37,43 @@
     <t>arrecadado_sucesso</t>
   </si>
   <si>
-    <t>media_sucesso</t>
-  </si>
-  <si>
-    <t>std_sucesso</t>
-  </si>
-  <si>
-    <t>min_sucesso</t>
-  </si>
-  <si>
-    <t>max_sucesso</t>
+    <t>arrecadado_avg</t>
+  </si>
+  <si>
+    <t>arrecadado_std</t>
+  </si>
+  <si>
+    <t>arrecadado_min</t>
+  </si>
+  <si>
+    <t>arrecadado_max</t>
   </si>
   <si>
     <t>apoio_medio</t>
   </si>
   <si>
+    <t>apoio_std</t>
+  </si>
+  <si>
+    <t>apoio_min</t>
+  </si>
+  <si>
+    <t>apoio_max</t>
+  </si>
+  <si>
     <t>contribuicoes</t>
   </si>
   <si>
-    <t>media_contribuicoes</t>
+    <t>contribuicoes_med</t>
+  </si>
+  <si>
+    <t>contribuicoes_std</t>
+  </si>
+  <si>
+    <t>contribuicoes_min</t>
+  </si>
+  <si>
+    <t>contribuicoes_max</t>
   </si>
   <si>
     <t>menor_ano</t>
@@ -445,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,11 +479,17 @@
     <col min="10" max="10" width="9.140625" style="3"/>
     <col min="11" max="11" width="9.140625" style="3"/>
     <col min="12" max="12" width="9.140625" style="3"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="13" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="9.140625" style="3"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="9.140625" style="1"/>
+    <col min="20" max="20" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:22">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -514,13 +538,31 @@
       <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1">
         <v>44</v>
@@ -550,27 +592,45 @@
         <v>111934.9031053756</v>
       </c>
       <c r="L2" s="3">
-        <v>94.08517009767365</v>
-      </c>
-      <c r="M2" s="1">
+        <v>94.9905854649608</v>
+      </c>
+      <c r="M2" s="3">
+        <v>47.6922463509549</v>
+      </c>
+      <c r="N2" s="3">
+        <v>47.35034461927121</v>
+      </c>
+      <c r="O2" s="3">
+        <v>305.2480444061168</v>
+      </c>
+      <c r="P2" s="1">
         <v>7547</v>
       </c>
-      <c r="N2" s="1">
+      <c r="Q2" s="1">
         <v>260.2413793103448</v>
       </c>
-      <c r="O2">
+      <c r="R2" s="1">
+        <v>212.2582078460797</v>
+      </c>
+      <c r="S2" s="1">
+        <v>35</v>
+      </c>
+      <c r="T2" s="1">
+        <v>808</v>
+      </c>
+      <c r="U2">
         <v>2012</v>
       </c>
-      <c r="P2">
+      <c r="V2">
         <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>117</v>
@@ -600,27 +660,45 @@
         <v>264585.9073482947</v>
       </c>
       <c r="L3" s="3">
-        <v>129.5537663642677</v>
-      </c>
-      <c r="M3" s="1">
+        <v>110.6538302669828</v>
+      </c>
+      <c r="M3" s="3">
+        <v>45.12744090621267</v>
+      </c>
+      <c r="N3" s="3">
+        <v>39.22956647121969</v>
+      </c>
+      <c r="O3" s="3">
+        <v>257.7853211115706</v>
+      </c>
+      <c r="P3" s="1">
         <v>32860</v>
       </c>
-      <c r="N3" s="1">
+      <c r="Q3" s="1">
         <v>395.9036144578313</v>
       </c>
-      <c r="O3">
+      <c r="R3" s="1">
+        <v>378.1809353534696</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1711</v>
+      </c>
+      <c r="U3">
         <v>2013</v>
       </c>
-      <c r="P3">
+      <c r="V3">
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1">
         <v>209</v>
@@ -650,27 +728,45 @@
         <v>537544.5528256212</v>
       </c>
       <c r="L4" s="3">
-        <v>79.80942858649695</v>
-      </c>
-      <c r="M4" s="1">
+        <v>82.69413375987617</v>
+      </c>
+      <c r="M4" s="3">
+        <v>30.90119243508478</v>
+      </c>
+      <c r="N4" s="3">
+        <v>13.93896149503088</v>
+      </c>
+      <c r="O4" s="3">
+        <v>194.2230576381307</v>
+      </c>
+      <c r="P4" s="1">
         <v>48629</v>
       </c>
-      <c r="N4" s="1">
+      <c r="Q4" s="1">
         <v>347.35</v>
       </c>
-      <c r="O4">
+      <c r="R4" s="1">
+        <v>547.4955526904555</v>
+      </c>
+      <c r="S4" s="1">
+        <v>3</v>
+      </c>
+      <c r="T4" s="1">
+        <v>5879</v>
+      </c>
+      <c r="U4">
         <v>2013</v>
       </c>
-      <c r="P4">
+      <c r="V4">
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1">
         <v>959</v>
@@ -700,27 +796,45 @@
         <v>679297.6600721752</v>
       </c>
       <c r="L5" s="3">
-        <v>87.19342470373856</v>
-      </c>
-      <c r="M5" s="1">
+        <v>91.3503645951285</v>
+      </c>
+      <c r="M5" s="3">
+        <v>52.58131393014926</v>
+      </c>
+      <c r="N5" s="3">
+        <v>21.61624650544615</v>
+      </c>
+      <c r="O5" s="3">
+        <v>792.0360759681182</v>
+      </c>
+      <c r="P5" s="1">
         <v>174471</v>
       </c>
-      <c r="N5" s="1">
+      <c r="Q5" s="1">
         <v>302.9010416666667</v>
       </c>
-      <c r="O5">
+      <c r="R5" s="1">
+        <v>401.4417134786221</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
+        <v>6494</v>
+      </c>
+      <c r="U5">
         <v>2011</v>
       </c>
-      <c r="P5">
+      <c r="V5">
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>6</v>
@@ -750,18 +864,36 @@
         <v>1720.659275370021</v>
       </c>
       <c r="L6" s="3">
-        <v>50.12134015913439</v>
-      </c>
-      <c r="M6" s="1">
+        <v>53.14416408875834</v>
+      </c>
+      <c r="M6" s="3">
+        <v>7.563317519432532</v>
+      </c>
+      <c r="N6" s="3">
+        <v>47.79609098250058</v>
+      </c>
+      <c r="O6" s="3">
+        <v>58.4922371950161</v>
+      </c>
+      <c r="P6" s="1">
         <v>46</v>
       </c>
-      <c r="N6" s="1">
+      <c r="Q6" s="1">
         <v>23</v>
       </c>
-      <c r="O6">
+      <c r="R6" s="1">
+        <v>18.38477631085023</v>
+      </c>
+      <c r="S6" s="1">
+        <v>10</v>
+      </c>
+      <c r="T6" s="1">
+        <v>36</v>
+      </c>
+      <c r="U6">
         <v>2012</v>
       </c>
-      <c r="P6">
+      <c r="V6">
         <v>2023</v>
       </c>
     </row>

</xml_diff>

<commit_message>
análise descritiva - acréscimo das metas
</commit_message>
<xml_diff>
--- a/analises/2023/analise_descritiva/dados/aon-genero.xlsx
+++ b/analises/2023/analise_descritiva/dados/aon-genero.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>modalidade</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>taxa_sucesso</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>meta_avg</t>
+  </si>
+  <si>
+    <t>meta_std</t>
+  </si>
+  <si>
+    <t>meta_min</t>
+  </si>
+  <si>
+    <t>meta_max</t>
   </si>
   <si>
     <t>arrecadado_sucesso</t>
@@ -463,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -482,14 +497,19 @@
     <col min="13" max="13" width="9.140625" style="3"/>
     <col min="14" max="14" width="9.140625" style="3"/>
     <col min="15" max="15" width="9.140625" style="3"/>
-    <col min="16" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="9.140625" style="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
+    <col min="16" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="9.140625" style="3"/>
+    <col min="18" max="18" width="9.140625" style="3"/>
+    <col min="19" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="9.140625" style="3"/>
+    <col min="21" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="9.140625" style="1"/>
+    <col min="23" max="23" width="9.140625" style="1"/>
+    <col min="24" max="24" width="9.140625" style="1"/>
+    <col min="25" max="25" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:27">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -556,13 +576,28 @@
       <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1">
         <v>44</v>
@@ -577,60 +612,75 @@
         <v>0.6590909090909091</v>
       </c>
       <c r="G2" s="3">
-        <v>710060.7787271431</v>
+        <v>495803.6844660074</v>
       </c>
       <c r="H2" s="3">
+        <v>17096.67877468991</v>
+      </c>
+      <c r="I2" s="3">
+        <v>15952.79958244942</v>
+      </c>
+      <c r="J2" s="3">
+        <v>3351.178010772499</v>
+      </c>
+      <c r="K2" s="3">
+        <v>61717.12812102117</v>
+      </c>
+      <c r="L2" s="3">
+        <v>710060.778727143</v>
+      </c>
+      <c r="M2" s="3">
         <v>24484.854438867</v>
       </c>
-      <c r="I2" s="3">
-        <v>25328.68179067508</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="N2" s="3">
+        <v>25328.68179067507</v>
+      </c>
+      <c r="O2" s="3">
         <v>4520.873062637543</v>
       </c>
-      <c r="K2" s="3">
+      <c r="P2" s="3">
         <v>111934.9031053756</v>
       </c>
-      <c r="L2" s="3">
+      <c r="Q2" s="3">
         <v>94.9905854649608</v>
       </c>
-      <c r="M2" s="3">
+      <c r="R2" s="3">
         <v>47.6922463509549</v>
       </c>
-      <c r="N2" s="3">
+      <c r="S2" s="3">
         <v>47.35034461927121</v>
       </c>
-      <c r="O2" s="3">
+      <c r="T2" s="3">
         <v>305.2480444061168</v>
       </c>
-      <c r="P2" s="1">
+      <c r="U2" s="1">
         <v>7547</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="V2" s="1">
         <v>260.2413793103448</v>
       </c>
-      <c r="R2" s="1">
+      <c r="W2" s="1">
         <v>212.2582078460797</v>
       </c>
-      <c r="S2" s="1">
+      <c r="X2" s="1">
         <v>35</v>
       </c>
-      <c r="T2" s="1">
+      <c r="Y2" s="1">
         <v>808</v>
       </c>
-      <c r="U2">
+      <c r="Z2">
         <v>2012</v>
       </c>
-      <c r="V2">
+      <c r="AA2">
         <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1">
         <v>117</v>
@@ -645,60 +695,75 @@
         <v>0.7094017094017094</v>
       </c>
       <c r="G3" s="3">
+        <v>2301598.727401814</v>
+      </c>
+      <c r="H3" s="3">
+        <v>27730.10514941945</v>
+      </c>
+      <c r="I3" s="3">
+        <v>34657.63167523112</v>
+      </c>
+      <c r="J3" s="3">
+        <v>46.55761904502517</v>
+      </c>
+      <c r="K3" s="3">
+        <v>189313.7035611726</v>
+      </c>
+      <c r="L3" s="3">
         <v>4257136.762729836</v>
       </c>
-      <c r="H3" s="3">
+      <c r="M3" s="3">
         <v>51290.80437023898</v>
       </c>
-      <c r="I3" s="3">
-        <v>65495.0813466783</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="N3" s="3">
+        <v>65495.08134667831</v>
+      </c>
+      <c r="O3" s="3">
         <v>54.53892516702949</v>
       </c>
-      <c r="K3" s="3">
+      <c r="P3" s="3">
         <v>264585.9073482947</v>
       </c>
-      <c r="L3" s="3">
+      <c r="Q3" s="3">
         <v>110.6538302669828</v>
       </c>
-      <c r="M3" s="3">
+      <c r="R3" s="3">
         <v>45.12744090621267</v>
       </c>
-      <c r="N3" s="3">
+      <c r="S3" s="3">
         <v>39.22956647121969</v>
       </c>
-      <c r="O3" s="3">
+      <c r="T3" s="3">
         <v>257.7853211115706</v>
       </c>
-      <c r="P3" s="1">
+      <c r="U3" s="1">
         <v>32860</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="V3" s="1">
         <v>395.9036144578313</v>
       </c>
-      <c r="R3" s="1">
+      <c r="W3" s="1">
         <v>378.1809353534696</v>
       </c>
-      <c r="S3" s="1">
+      <c r="X3" s="1">
         <v>1</v>
       </c>
-      <c r="T3" s="1">
+      <c r="Y3" s="1">
         <v>1711</v>
       </c>
-      <c r="U3">
+      <c r="Z3">
         <v>2013</v>
       </c>
-      <c r="V3">
+      <c r="AA3">
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
         <v>209</v>
@@ -713,60 +778,75 @@
         <v>0.6698564593301436</v>
       </c>
       <c r="G4" s="3">
-        <v>3881052.70273276</v>
+        <v>2221303.500608701</v>
       </c>
       <c r="H4" s="3">
+        <v>15866.45357577644</v>
+      </c>
+      <c r="I4" s="3">
+        <v>11237.67595303987</v>
+      </c>
+      <c r="J4" s="3">
+        <v>31.89582864100442</v>
+      </c>
+      <c r="K4" s="3">
+        <v>80883.37226400203</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3881052.702732761</v>
+      </c>
+      <c r="M4" s="3">
         <v>27721.80501951972</v>
       </c>
-      <c r="I4" s="3">
+      <c r="N4" s="3">
         <v>48958.87135925953</v>
       </c>
-      <c r="J4" s="3">
+      <c r="O4" s="3">
         <v>41.81688448509265</v>
       </c>
-      <c r="K4" s="3">
+      <c r="P4" s="3">
         <v>537544.5528256212</v>
       </c>
-      <c r="L4" s="3">
-        <v>82.69413375987617</v>
-      </c>
-      <c r="M4" s="3">
+      <c r="Q4" s="3">
+        <v>82.69413375987618</v>
+      </c>
+      <c r="R4" s="3">
         <v>30.90119243508478</v>
       </c>
-      <c r="N4" s="3">
+      <c r="S4" s="3">
         <v>13.93896149503088</v>
       </c>
-      <c r="O4" s="3">
+      <c r="T4" s="3">
         <v>194.2230576381307</v>
       </c>
-      <c r="P4" s="1">
+      <c r="U4" s="1">
         <v>48629</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="V4" s="1">
         <v>347.35</v>
       </c>
-      <c r="R4" s="1">
+      <c r="W4" s="1">
         <v>547.4955526904555</v>
       </c>
-      <c r="S4" s="1">
+      <c r="X4" s="1">
         <v>3</v>
       </c>
-      <c r="T4" s="1">
+      <c r="Y4" s="1">
         <v>5879</v>
       </c>
-      <c r="U4">
+      <c r="Z4">
         <v>2013</v>
       </c>
-      <c r="V4">
+      <c r="AA4">
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:27">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>959</v>
@@ -781,60 +861,75 @@
         <v>0.6006256517205423</v>
       </c>
       <c r="G5" s="3">
+        <v>8952422.29225223</v>
+      </c>
+      <c r="H5" s="3">
+        <v>15542.3998129379</v>
+      </c>
+      <c r="I5" s="3">
+        <v>13538.7952845963</v>
+      </c>
+      <c r="J5" s="3">
+        <v>33.25544217501798</v>
+      </c>
+      <c r="K5" s="3">
+        <v>80687.35013615266</v>
+      </c>
+      <c r="L5" s="3">
         <v>15212724.00148597</v>
       </c>
-      <c r="H5" s="3">
-        <v>26410.97916924648</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="M5" s="3">
+        <v>26410.97916924647</v>
+      </c>
+      <c r="N5" s="3">
         <v>40119.88399963382</v>
       </c>
-      <c r="J5" s="3">
+      <c r="O5" s="3">
         <v>94.898114598278</v>
       </c>
-      <c r="K5" s="3">
+      <c r="P5" s="3">
         <v>679297.6600721752</v>
       </c>
-      <c r="L5" s="3">
+      <c r="Q5" s="3">
         <v>91.3503645951285</v>
       </c>
-      <c r="M5" s="3">
+      <c r="R5" s="3">
         <v>52.58131393014926</v>
       </c>
-      <c r="N5" s="3">
+      <c r="S5" s="3">
         <v>21.61624650544615</v>
       </c>
-      <c r="O5" s="3">
+      <c r="T5" s="3">
         <v>792.0360759681182</v>
       </c>
-      <c r="P5" s="1">
+      <c r="U5" s="1">
         <v>174471</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="V5" s="1">
         <v>302.9010416666667</v>
       </c>
-      <c r="R5" s="1">
+      <c r="W5" s="1">
         <v>401.4417134786221</v>
       </c>
-      <c r="S5" s="1">
+      <c r="X5" s="1">
         <v>1</v>
       </c>
-      <c r="T5" s="1">
+      <c r="Y5" s="1">
         <v>6494</v>
       </c>
-      <c r="U5">
+      <c r="Z5">
         <v>2011</v>
       </c>
-      <c r="V5">
+      <c r="AA5">
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:27">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
         <v>6</v>
@@ -849,51 +944,66 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="G6" s="3">
+        <v>1914.395463895744</v>
+      </c>
+      <c r="H6" s="3">
+        <v>957.1977319478718</v>
+      </c>
+      <c r="I6" s="3">
+        <v>774.6384084502962</v>
+      </c>
+      <c r="J6" s="3">
+        <v>409.4456603651128</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1504.949803530631</v>
+      </c>
+      <c r="L6" s="3">
         <v>2305.581647320182</v>
       </c>
-      <c r="H6" s="3">
+      <c r="M6" s="3">
         <v>1152.790823660091</v>
       </c>
-      <c r="I6" s="3">
+      <c r="N6" s="3">
         <v>803.0872660519939</v>
       </c>
-      <c r="J6" s="3">
+      <c r="O6" s="3">
         <v>584.9223719501611</v>
       </c>
-      <c r="K6" s="3">
+      <c r="P6" s="3">
         <v>1720.659275370021</v>
       </c>
-      <c r="L6" s="3">
+      <c r="Q6" s="3">
         <v>53.14416408875834</v>
       </c>
-      <c r="M6" s="3">
+      <c r="R6" s="3">
         <v>7.563317519432532</v>
       </c>
-      <c r="N6" s="3">
+      <c r="S6" s="3">
         <v>47.79609098250058</v>
       </c>
-      <c r="O6" s="3">
+      <c r="T6" s="3">
         <v>58.4922371950161</v>
       </c>
-      <c r="P6" s="1">
+      <c r="U6" s="1">
         <v>46</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="V6" s="1">
         <v>23</v>
       </c>
-      <c r="R6" s="1">
+      <c r="W6" s="1">
         <v>18.38477631085023</v>
       </c>
-      <c r="S6" s="1">
+      <c r="X6" s="1">
         <v>10</v>
       </c>
-      <c r="T6" s="1">
+      <c r="Y6" s="1">
         <v>36</v>
       </c>
-      <c r="U6">
+      <c r="Z6">
         <v>2012</v>
       </c>
-      <c r="V6">
+      <c r="AA6">
         <v>2023</v>
       </c>
     </row>

</xml_diff>